<commit_message>
Updated script and tests
</commit_message>
<xml_diff>
--- a/ProvarProject/templates/TestData.xlsx
+++ b/ProvarProject/templates/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\provardx\ProvarProject\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\STARWEST\provar_demo\ProvarProject\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD9F04A-8A37-4C66-B5BF-C899B5F01B33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC5C65A-88B3-424C-A6BD-B950EDEBBD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4050" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="18224" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -555,7 +555,7 @@
         <v>24</v>
       </c>
       <c r="O2" s="1">
-        <v>43831</v>
+        <v>44075</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +569,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:D2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>